<commit_message>
Generate nuclet from xlsx
git-svn-id: https://svn.novabit.de/nov_nucleus/trunk@7760 33553225-e83a-40c5-8946-3093c540bf14
</commit_message>
<xml_diff>
--- a/nuclos-client/src/main/resources/org/nuclos/client/nuclet/generator/NucletGeneration.xlsx
+++ b/nuclos-client/src/main/resources/org/nuclos/client/nuclet/generator/NucletGeneration.xlsx
@@ -13,11 +13,34 @@
     <sheet name="_(Version)_" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Maik Stüker</author>
+  </authors>
+  <commentList>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ALT = 8
+CTRL = 2</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Maik Stüker</author>
@@ -45,7 +68,6 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
@@ -61,7 +83,6 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
@@ -75,7 +96,6 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
@@ -92,7 +112,6 @@
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
@@ -109,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>1.0</t>
   </si>
@@ -321,6 +340,21 @@
   </si>
   <si>
     <t>Nullable</t>
+  </si>
+  <si>
+    <t>Accelerator</t>
+  </si>
+  <si>
+    <t>Char (1)</t>
+  </si>
+  <si>
+    <t>Accelerator Modifier</t>
+  </si>
+  <si>
+    <t>Number (2)</t>
+  </si>
+  <si>
+    <t>Menushortcut</t>
   </si>
 </sst>
 </file>
@@ -357,13 +391,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -376,6 +403,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -419,11 +452,11 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -724,11 +757,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
@@ -739,19 +772,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="34.140625" customWidth="1"/>
     <col min="4" max="4" width="46.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -765,28 +801,37 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -800,13 +845,13 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>3</v>
@@ -815,12 +860,22 @@
         <v>3</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -832,7 +887,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
@@ -1019,7 +1074,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>